<commit_message>
75: Separate Investigated and Easy Methods
Task-Url: http://github.com/llmhyy/evosuite_progress/issues/75
</commit_message>
<xml_diff>
--- a/EvosuiteTest/experiments/SF100/reports/interprocedure-flag-problem-distribution.xlsx
+++ b/EvosuiteTest/experiments/SF100/reports/interprocedure-flag-problem-distribution.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lylytran/Projects/Evosuite/modified-version/evosuite/EvosuiteTest/experiments/SF100/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linyun\Documents\git_space\evosuite\EvosuiteTest\experiments\SF100\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8521901-B4CB-42D4-96ED-8125252543B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16420"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">data!$E$2:$E$99</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">data!$E$2:$E$99</definedName>
+  </definedNames>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -635,7 +640,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -677,8 +682,684 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{51AA7FE4-6A4E-464A-B859-B2DD28EE26D5}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>73478</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>263978</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117021</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E52C2B6B-1A3C-4F1B-AB0A-7DB1311BE83B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4454978" y="704850"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-SG" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -943,16 +1624,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E99" sqref="E2:E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -969,7 +1650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -986,7 +1667,7 @@
         <v>0.81666665999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1684,7 @@
         <v>0.11206896600000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1020,7 +1701,7 @@
         <v>0.38235295000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1718,7 @@
         <v>0.31111112000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1054,7 +1735,7 @@
         <v>0.23913044</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1071,7 +1752,7 @@
         <v>0.44074073000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1088,7 +1769,7 @@
         <v>0.31578946000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1786,7 @@
         <v>0.27631578000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1122,7 +1803,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1139,7 +1820,7 @@
         <v>0.26470589999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1156,7 +1837,7 @@
         <v>0.44444444999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1173,7 +1854,7 @@
         <v>0.68292682999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1190,7 +1871,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1207,7 +1888,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1224,7 +1905,7 @@
         <v>0.55319149999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1241,7 +1922,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1258,7 +1939,7 @@
         <v>0.17460318</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1275,7 +1956,7 @@
         <v>0.5642857</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1292,7 +1973,7 @@
         <v>0.33862432999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1309,7 +1990,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1326,7 +2007,7 @@
         <v>9.3333334000000004E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1343,7 +2024,7 @@
         <v>0.33333333999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1360,7 +2041,7 @@
         <v>0.5533981</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1377,7 +2058,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1394,7 +2075,7 @@
         <v>0.19047620000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1411,7 +2092,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +2109,7 @@
         <v>0.34166667000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -1445,7 +2126,7 @@
         <v>0.32038834999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1462,7 +2143,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1479,7 +2160,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1496,7 +2177,7 @@
         <v>0.44444444999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -1513,7 +2194,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -1530,7 +2211,7 @@
         <v>0.35632184</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1547,7 +2228,7 @@
         <v>0.3783784</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -1564,7 +2245,7 @@
         <v>0.48559671999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1581,7 +2262,7 @@
         <v>0.30769232000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -1598,7 +2279,7 @@
         <v>0.56218904000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -1615,7 +2296,7 @@
         <v>0.14285714999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -1632,7 +2313,7 @@
         <v>0.48235294000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -1649,7 +2330,7 @@
         <v>0.4225352</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -1666,7 +2347,7 @@
         <v>0.44444444999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -1683,7 +2364,7 @@
         <v>0.47579529999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -1700,7 +2381,7 @@
         <v>0.47286244999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -1717,7 +2398,7 @@
         <v>0.57692310000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -1734,7 +2415,7 @@
         <v>0.72027969999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -1751,7 +2432,7 @@
         <v>0.73333334999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -1768,7 +2449,7 @@
         <v>0.54054049999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -1785,7 +2466,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -1802,7 +2483,7 @@
         <v>0.33333333999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -1819,7 +2500,7 @@
         <v>0.21254355</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -1836,7 +2517,7 @@
         <v>0.46153845999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -1853,7 +2534,7 @@
         <v>0.33333333999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -1870,7 +2551,7 @@
         <v>0.70769230000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -1887,7 +2568,7 @@
         <v>0.47368421999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -1904,7 +2585,7 @@
         <v>0.46341463999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -1921,7 +2602,7 @@
         <v>0.52659579999999995</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>117</v>
       </c>
@@ -1938,7 +2619,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -1955,7 +2636,7 @@
         <v>0.15238096000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>121</v>
       </c>
@@ -1972,7 +2653,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -1989,7 +2670,7 @@
         <v>0.17647060000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -2006,7 +2687,7 @@
         <v>0.33078099999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>127</v>
       </c>
@@ -2023,7 +2704,7 @@
         <v>0.46060606999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>129</v>
       </c>
@@ -2040,7 +2721,7 @@
         <v>0.19402985</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>131</v>
       </c>
@@ -2057,7 +2738,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -2074,7 +2755,7 @@
         <v>0.22929542999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>135</v>
       </c>
@@ -2091,7 +2772,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>137</v>
       </c>
@@ -2108,7 +2789,7 @@
         <v>0.26136363000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>139</v>
       </c>
@@ -2125,7 +2806,7 @@
         <v>0.42949757</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>141</v>
       </c>
@@ -2142,7 +2823,7 @@
         <v>0.62962960000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>143</v>
       </c>
@@ -2159,7 +2840,7 @@
         <v>0.40384614000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>145</v>
       </c>
@@ -2176,7 +2857,7 @@
         <v>0.39285713</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>147</v>
       </c>
@@ -2193,7 +2874,7 @@
         <v>0.43037975000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>149</v>
       </c>
@@ -2210,7 +2891,7 @@
         <v>0.28571429999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>151</v>
       </c>
@@ -2227,7 +2908,7 @@
         <v>0.3955224</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>153</v>
       </c>
@@ -2244,7 +2925,7 @@
         <v>0.47222219999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>155</v>
       </c>
@@ -2261,7 +2942,7 @@
         <v>0.47058823999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -2278,7 +2959,7 @@
         <v>0.26228538000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>159</v>
       </c>
@@ -2295,7 +2976,7 @@
         <v>0.47552450000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>161</v>
       </c>
@@ -2312,7 +2993,7 @@
         <v>0.40262583000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>163</v>
       </c>
@@ -2329,7 +3010,7 @@
         <v>0.37931034000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>165</v>
       </c>
@@ -2346,7 +3027,7 @@
         <v>0.43478260000000002</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>167</v>
       </c>
@@ -2363,7 +3044,7 @@
         <v>0.25599050000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>169</v>
       </c>
@@ -2380,7 +3061,7 @@
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>171</v>
       </c>
@@ -2397,7 +3078,7 @@
         <v>0.53900707000000003</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>173</v>
       </c>
@@ -2414,7 +3095,7 @@
         <v>0.52727270000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>175</v>
       </c>
@@ -2431,7 +3112,7 @@
         <v>0.23809524000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>177</v>
       </c>
@@ -2448,7 +3129,7 @@
         <v>3.2348804000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>179</v>
       </c>
@@ -2465,7 +3146,7 @@
         <v>0.44444444999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>181</v>
       </c>
@@ -2482,7 +3163,7 @@
         <v>0.41379312000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>183</v>
       </c>
@@ -2499,7 +3180,7 @@
         <v>0.49425286000000002</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>185</v>
       </c>
@@ -2516,7 +3197,7 @@
         <v>0.34426230000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>187</v>
       </c>
@@ -2533,7 +3214,7 @@
         <v>0.57142859999999995</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>189</v>
       </c>
@@ -2550,7 +3231,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>191</v>
       </c>
@@ -2567,7 +3248,7 @@
         <v>0.34679335</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>193</v>
       </c>
@@ -2584,7 +3265,7 @@
         <v>0.52857140000000002</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>195</v>
       </c>
@@ -2601,7 +3282,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>197</v>
       </c>
@@ -2618,7 +3299,7 @@
         <v>0.44036698000000002</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>199</v>
       </c>
@@ -2635,7 +3316,7 @@
         <v>0.57894736999999996</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C100">
         <f>SUM(C2:C99)</f>
         <v>21182</v>
@@ -2651,5 +3332,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>